<commit_message>
fix: remove newlines from simple texts (DEV-5007) (#39)
</commit_message>
<xml_diff>
--- a/data/spreadsheets/BookCover.xlsx
+++ b/data/spreadsheets/BookCover.xlsx
@@ -1,21 +1,34 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10420"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10526"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/noemivillars-amberg/Documents/daschland-scripts/data/Spreadsheet_Data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nussbaum/Desktop/Cloned_GitHub_repos/daschland-scripts/data/spreadsheets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{594ED468-8E20-9F4C-98EF-8DEBF524D71B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA8F4DD3-4A8D-BB48-B902-F725ECAD4F07}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13100" yWindow="500" windowWidth="60500" windowHeight="22900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="21580" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0" iterateDelta="1E-4"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -119,10 +132,6 @@
 5 p. l., 133 p. col. front., illus. (part col.) col. plates. 23 cm. </t>
   </si>
   <si>
-    <t>The books in this collection are in the public domain and are free to use and reuse.
-Credit Line: Library of Congress</t>
-  </si>
-  <si>
     <r>
       <rPr>
         <u/>
@@ -323,6 +332,9 @@
   </si>
   <si>
     <t>Public Domain</t>
+  </si>
+  <si>
+    <t>The books in this collection are in the public domain and are free to use and reuse. Credit Line: Library of Congress</t>
   </si>
 </sst>
 </file>
@@ -1526,8 +1538,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I8"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1565,18 +1577,18 @@
         <v>5</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="H1" s="2" t="s">
         <v>6</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>7</v>
@@ -1585,16 +1597,16 @@
         <v>8</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F2" s="2" t="s">
         <v>9</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="H2" s="2" t="s">
         <v>10</v>
@@ -1605,7 +1617,7 @@
     </row>
     <row r="3" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>12</v>
@@ -1617,13 +1629,13 @@
         <v>14</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F3" s="2" t="s">
         <v>15</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="H3" s="2" t="s">
         <v>16</v>
@@ -1632,9 +1644,9 @@
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="51" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>18</v>
@@ -1646,135 +1658,135 @@
         <v>20</v>
       </c>
       <c r="E4" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="F4" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="F4" s="3" t="s">
+      <c r="G4" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="H4" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="G4" s="2" t="s">
+      <c r="I4" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="34" x14ac:dyDescent="0.2">
+      <c r="A5" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="H5" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="I5" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="34" x14ac:dyDescent="0.2">
+      <c r="A6" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="D6" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="H4" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="I4" s="2" t="s">
-        <v>23</v>
+      <c r="E6" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="H6" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="I6" s="2" t="s">
+        <v>31</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="51" x14ac:dyDescent="0.2">
-      <c r="A5" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="E5" s="2" t="s">
+    <row r="7" spans="1:9" ht="34" x14ac:dyDescent="0.2">
+      <c r="A7" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="F7" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="F5" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="G5" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="H5" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="I5" s="2" t="s">
-        <v>28</v>
+      <c r="G7" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="H7" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="I7" s="2" t="s">
+        <v>34</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="51" x14ac:dyDescent="0.2">
-      <c r="A6" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="E6" s="2" t="s">
+    <row r="8" spans="1:9" ht="34" x14ac:dyDescent="0.2">
+      <c r="A8" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="F8" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="F6" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="G6" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="H6" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="I6" s="2" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" ht="51" x14ac:dyDescent="0.2">
-      <c r="A7" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="E7" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="F7" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="G7" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="H7" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="I7" s="2" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" ht="51" x14ac:dyDescent="0.2">
-      <c r="A8" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="D8" s="3" t="s">
+      <c r="G8" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="H8" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="E8" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="F8" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="G8" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="H8" s="2" t="s">
+      <c r="I8" s="2" t="s">
         <v>39</v>
-      </c>
-      <c r="I8" s="2" t="s">
-        <v>40</v>
       </c>
     </row>
   </sheetData>

</xml_diff>